<commit_message>
add api definitions in docs, just for tenant/product/device
</commit_message>
<xml_diff>
--- a/docs/iot_apis.xlsx
+++ b/docs/iot_apis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="27900" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="30100" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="143">
   <si>
     <t>Api</t>
   </si>
@@ -387,6 +387,75 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Tenant</t>
+  </si>
+  <si>
+    <t>POST /tenants/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>Delete Tenant</t>
+  </si>
+  <si>
+    <t>Add Tenant</t>
+  </si>
+  <si>
+    <t>DELETE /tenants/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>Delete a tenant from IoT cloud</t>
+  </si>
+  <si>
+    <t>Add a tenant to IoT cloud</t>
+  </si>
+  <si>
+    <t>Get Tenant details</t>
+  </si>
+  <si>
+    <t>GET /tenants/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>Get tenant detail from IoT cloud</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Add Product</t>
+  </si>
+  <si>
+    <t>Delete Product</t>
+  </si>
+  <si>
+    <t>Add product</t>
+  </si>
+  <si>
+    <t>POST /products/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /products/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>Delete product</t>
+  </si>
+  <si>
+    <t>Get Product Info</t>
+  </si>
+  <si>
+    <t>GET /products/{id}?version=v1</t>
+  </si>
+  <si>
+    <t>Get product information from iot cloud</t>
+  </si>
+  <si>
+    <t>Get Product device list</t>
+  </si>
+  <si>
+    <t>GET /products/{id}?/devices?version=v1</t>
+  </si>
+  <si>
+    <t>Get product devices list</t>
   </si>
 </sst>
 </file>
@@ -416,7 +485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -601,17 +670,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -637,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -660,6 +718,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -671,21 +741,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,19 +1019,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I55"/>
+  <dimension ref="B1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="52.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="25.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="64.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="47" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="36.33203125" style="1" customWidth="1"/>
@@ -986,868 +1041,946 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="2:9" ht="68" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8">
+        <f>B3+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8">
+        <f t="shared" ref="B5:B10" si="0">B4+1</f>
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="2:9" ht="33" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" s="15">
-        <f>B4+1</f>
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B6" s="15">
-        <f t="shared" ref="B6:B44" si="0">B5+1</f>
+      <c r="C5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="8">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B7" s="15">
+      <c r="C6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="15">
+      <c r="C7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B9" s="15">
+      <c r="C8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="15">
+      <c r="C9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
+        <f>B10+1</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B11" s="15">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8">
+        <f>B11+1</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B12" s="15">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="15">
-        <f t="shared" si="0"/>
+    <row r="13" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8">
+        <f t="shared" ref="B13:B46" si="1">B12+1</f>
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="15">
-        <f t="shared" si="0"/>
+    <row r="14" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="15">
-        <f t="shared" si="0"/>
+    <row r="15" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="8">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="15">
-        <f t="shared" si="0"/>
+    <row r="16" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="8">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="15">
-        <f t="shared" si="0"/>
+    <row r="17" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="8">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="15">
-        <f t="shared" si="0"/>
+    <row r="18" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B19" s="15">
-        <f t="shared" si="0"/>
+    <row r="19" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="8">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="15">
-        <f t="shared" si="0"/>
+    <row r="20" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="8">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B21" s="15">
-        <f t="shared" si="0"/>
+    <row r="21" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B22" s="15">
-        <f t="shared" si="0"/>
+    <row r="22" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="8">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B23" s="15">
-        <f t="shared" si="0"/>
+    <row r="23" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B24" s="15">
-        <f t="shared" si="0"/>
+    <row r="24" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="8">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="B25" s="15">
-        <f t="shared" si="0"/>
+    <row r="25" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B26" s="15">
-        <f t="shared" si="0"/>
+    <row r="26" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="8">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B27" s="15">
-        <f t="shared" si="0"/>
+    <row r="27" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="8">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B28" s="15">
-        <f t="shared" si="0"/>
+    <row r="28" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="8">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="B29" s="15">
-        <f t="shared" si="0"/>
+    <row r="29" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="8">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B30" s="15">
-        <f t="shared" si="0"/>
+    <row r="30" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="8">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="15">
-        <f t="shared" si="0"/>
+    <row r="31" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B32" s="15">
-        <f t="shared" si="0"/>
+    <row r="32" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="8">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B33" s="15">
-        <f t="shared" si="0"/>
+    <row r="33" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="8">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B34" s="15">
-        <f t="shared" si="0"/>
+    <row r="34" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="8">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B35" s="15">
-        <f t="shared" si="0"/>
+    <row r="35" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="8">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B36" s="15">
-        <f t="shared" si="0"/>
+    <row r="36" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="8">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B37" s="15">
-        <f t="shared" si="0"/>
+    <row r="37" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="8">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="15">
-        <f t="shared" si="0"/>
+    <row r="38" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="8">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B39" s="15">
-        <f t="shared" si="0"/>
+    <row r="39" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="8">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="15"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+    <row r="40" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="15"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+    <row r="41" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="8">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="15"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+    <row r="42" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="8">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="15"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+    <row r="43" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="15"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+    <row r="44" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="8">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="15"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+    <row r="45" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="8">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="15"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+    <row r="46" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="15"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1857,7 +1990,7 @@
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="15"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1867,7 +2000,7 @@
       <c r="I48" s="3"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="15"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1877,7 +2010,7 @@
       <c r="I49" s="3"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1887,7 +2020,7 @@
       <c r="I50" s="3"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1897,7 +2030,7 @@
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B52" s="15"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1907,7 +2040,7 @@
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="15"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1917,7 +2050,7 @@
       <c r="I53" s="3"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1926,23 +2059,93 @@
       <c r="H54" s="2"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="16"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="5"/>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="8"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="8"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="8"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="8"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="8"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="8"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="8"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>

</xml_diff>

<commit_message>
add changes for product apis
</commit_message>
<xml_diff>
--- a/docs/iot_apis.xlsx
+++ b/docs/iot_apis.xlsx
@@ -284,126 +284,21 @@
     <t>This method is used to notify an IoT hub of a completed file upload</t>
   </si>
   <si>
-    <t>POST /devices?version=v1</t>
-  </si>
-  <si>
-    <t>DELETE /devices/{id}?version=v1</t>
-  </si>
-  <si>
-    <t>GET /devices/{id}?version=v1</t>
-  </si>
-  <si>
-    <t>GET /devices?version=v1&amp;top={top}</t>
-  </si>
-  <si>
-    <t>GET /statistics/devices?version=v1</t>
-  </si>
-  <si>
-    <t>GET /statistics/service?version=v1</t>
-  </si>
-  <si>
-    <t>DELETE /devices/{id}/commands?version=v1</t>
-  </si>
-  <si>
-    <t>PUT /devices/{id}?version=v1</t>
-  </si>
-  <si>
-    <t>POST /devices/query?version=v1</t>
-  </si>
-  <si>
-    <t>GET /twins/{id}?version=v1</t>
-  </si>
-  <si>
-    <t>POST /twins/{id}/methods?version=v1</t>
-  </si>
-  <si>
-    <t>PATCH /twins/{id}?version=v1</t>
-  </si>
-  <si>
     <t>GET /jobs/v2/{jobid}</t>
   </si>
   <si>
-    <t>POST /subscriptions/{subscriptionId}/nameAvailability?version=v1</t>
-  </si>
-  <si>
-    <t>DELETE /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?aversion=v1</t>
-  </si>
-  <si>
-    <t>PUT /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?version=v1</t>
-  </si>
-  <si>
-    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/exportDevices?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/jobs/{jobId}?version=v1</t>
-  </si>
-  <si>
-    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/hubKeys/{keyName}/listkeys?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/quotaMetrics?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/skus?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/stats?version=v1</t>
-  </si>
-  <si>
-    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/providers/hubs/{resourceName}/importDevices?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/hubs?version=v1</t>
-  </si>
-  <si>
-    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/jobs?version=v1</t>
-  </si>
-  <si>
-    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/listkeys?version=v1</t>
-  </si>
-  <si>
-    <t>POST /devices/{id}/messages/deviceBound/{etag}/abandon?version=v1</t>
-  </si>
-  <si>
-    <t>DELETE /devices/{id}/messages/deviceBound/{etag}?version=v1&amp;reject={reject}</t>
-  </si>
-  <si>
-    <t>POST /devices/{deviceId}/files?version=v1</t>
-  </si>
-  <si>
-    <t>GET /devices/{id}/messages/deviceBound?version=v1</t>
-  </si>
-  <si>
-    <t>POST /devices/{id}/messages/events?version=v1</t>
-  </si>
-  <si>
-    <t>POST /devices/{deviceId}/files/notifications?version=v1</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Tenant</t>
   </si>
   <si>
-    <t>POST /tenants/{id}?version=v1</t>
-  </si>
-  <si>
     <t>Delete Tenant</t>
   </si>
   <si>
     <t>Add Tenant</t>
   </si>
   <si>
-    <t>DELETE /tenants/{id}?version=v1</t>
-  </si>
-  <si>
     <t>Delete a tenant from IoT cloud</t>
   </si>
   <si>
@@ -413,9 +308,6 @@
     <t>Get Tenant details</t>
   </si>
   <si>
-    <t>GET /tenants/{id}?version=v1</t>
-  </si>
-  <si>
     <t>Get tenant detail from IoT cloud</t>
   </si>
   <si>
@@ -431,31 +323,139 @@
     <t>Add product</t>
   </si>
   <si>
-    <t>POST /products/{id}?version=v1</t>
-  </si>
-  <si>
-    <t>DELETE /products/{id}?version=v1</t>
-  </si>
-  <si>
     <t>Delete product</t>
   </si>
   <si>
     <t>Get Product Info</t>
   </si>
   <si>
-    <t>GET /products/{id}?version=v1</t>
-  </si>
-  <si>
     <t>Get product information from iot cloud</t>
   </si>
   <si>
     <t>Get Product device list</t>
   </si>
   <si>
-    <t>GET /products/{id}?/devices?version=v1</t>
-  </si>
-  <si>
     <t>Get product devices list</t>
+  </si>
+  <si>
+    <t>POST /tenants/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /tenants/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /tenants/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /products/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /products/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /products/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /products/{id}?/devices?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /devices?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /devices/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /devices/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /devices?api-version=v1&amp;top={top}</t>
+  </si>
+  <si>
+    <t>GET /statistics/devices?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /statistics/service?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /devices/{id}/commands?api-version=v1</t>
+  </si>
+  <si>
+    <t>PUT /devices/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /devices/query?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /twins/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /twins/{id}/methods?api-version=v1</t>
+  </si>
+  <si>
+    <t>PATCH /twins/{id}?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /subscriptions/{subscriptionId}/nameAvailability?api-version=v1</t>
+  </si>
+  <si>
+    <t>PUT /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?aapi-version=v1</t>
+  </si>
+  <si>
+    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/exportDevices?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/jobs/{jobId}?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/hubKeys/{keyName}/listkeys?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/quotaMetrics?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/stats?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/skus?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/providers/hubs/{resourceName}/importDevices?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/hubs?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/jobs?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/hubs/{resourceName}/listkeys?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /devices/{id}/messages/deviceBound/{etag}/abandon?api-version=v1</t>
+  </si>
+  <si>
+    <t>DELETE /devices/{id}/messages/deviceBound/{etag}?api-version=v1&amp;reject={reject}</t>
+  </si>
+  <si>
+    <t>POST /devices/{deviceId}/files?api-version=v1</t>
+  </si>
+  <si>
+    <t>GET /devices/{id}/messages/deviceBound?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /devices/{id}/messages/events?api-version=v1</t>
+  </si>
+  <si>
+    <t>POST /devices/{deviceId}/files/notifications?api-version=v1</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +481,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -741,6 +747,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,7 +1037,7 @@
   <dimension ref="B1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1057,7 @@
     <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>2</v>
@@ -1082,16 +1097,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1103,16 +1118,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1124,104 +1139,104 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="8">
+      <c r="B7" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
+      <c r="C7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8">
+      <c r="B8" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
+      <c r="C8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="8">
+      <c r="B9" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+      <c r="C9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
+      <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="C10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="2:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
@@ -1235,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>16</v>
@@ -1256,7 +1271,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>18</v>
@@ -1277,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>20</v>
@@ -1298,7 +1313,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
@@ -1319,7 +1334,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>24</v>
@@ -1340,7 +1355,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>26</v>
@@ -1361,7 +1376,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>28</v>
@@ -1382,7 +1397,7 @@
         <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>30</v>
@@ -1403,7 +1418,7 @@
         <v>31</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>32</v>
@@ -1424,7 +1439,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>35</v>
@@ -1445,7 +1460,7 @@
         <v>37</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>36</v>
@@ -1466,7 +1481,7 @@
         <v>39</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>38</v>
@@ -1529,7 +1544,7 @@
         <v>48</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>47</v>
@@ -1550,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>6</v>
@@ -1571,7 +1586,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>10</v>
@@ -1592,7 +1607,7 @@
         <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>13</v>
@@ -1613,7 +1628,7 @@
         <v>50</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>49</v>
@@ -1634,7 +1649,7 @@
         <v>51</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>52</v>
@@ -1655,7 +1670,7 @@
         <v>48</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>53</v>
@@ -1676,7 +1691,7 @@
         <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>54</v>
@@ -1697,7 +1712,7 @@
         <v>57</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>56</v>
@@ -1718,7 +1733,7 @@
         <v>59</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>58</v>
@@ -1739,7 +1754,7 @@
         <v>61</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>60</v>
@@ -1760,7 +1775,7 @@
         <v>62</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>63</v>
@@ -1781,7 +1796,7 @@
         <v>65</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>64</v>
@@ -1802,7 +1817,7 @@
         <v>67</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>66</v>
@@ -1823,7 +1838,7 @@
         <v>69</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>68</v>
@@ -1844,7 +1859,7 @@
         <v>71</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>70</v>
@@ -1865,7 +1880,7 @@
         <v>72</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>74</v>
@@ -1886,7 +1901,7 @@
         <v>75</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>76</v>
@@ -1907,7 +1922,7 @@
         <v>77</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>81</v>
@@ -1928,7 +1943,7 @@
         <v>78</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>82</v>
@@ -1949,7 +1964,7 @@
         <v>79</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>83</v>
@@ -1970,7 +1985,7 @@
         <v>80</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>84</v>

</xml_diff>